<commit_message>
adding tostring for card
</commit_message>
<xml_diff>
--- a/assets/cards.xlsx
+++ b/assets/cards.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\mycode\blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{040BB83C-37C6-49DE-88A8-D4617FCE1FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4184BF45-B535-4E35-A175-A14F971C1B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{577205D3-06DB-45CE-85F4-7344C670B98B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="69">
   <si>
     <t>Diamond</t>
   </si>
@@ -87,23 +88,185 @@
     <t>King</t>
   </si>
   <si>
-    <t>cardsToTest.Add(new Card { Suit = CardSuit.Diamond,Value = CardValue.Ace});</t>
-  </si>
-  <si>
     <t>cardsToTest.Add(new Card { Suit = CardSuit.</t>
+  </si>
+  <si>
+    <t>🂡</t>
+  </si>
+  <si>
+    <t>🂢</t>
+  </si>
+  <si>
+    <t>🂣</t>
+  </si>
+  <si>
+    <t>🂤</t>
+  </si>
+  <si>
+    <t>🂱</t>
+  </si>
+  <si>
+    <t>🂲</t>
+  </si>
+  <si>
+    <t>🂳</t>
+  </si>
+  <si>
+    <t>🂴</t>
+  </si>
+  <si>
+    <t>🂵</t>
+  </si>
+  <si>
+    <t>🂶</t>
+  </si>
+  <si>
+    <t>🂷</t>
+  </si>
+  <si>
+    <t>🂸</t>
+  </si>
+  <si>
+    <t>🂹</t>
+  </si>
+  <si>
+    <t>🂺</t>
+  </si>
+  <si>
+    <t>🂻</t>
+  </si>
+  <si>
+    <t>🂽</t>
+  </si>
+  <si>
+    <t>🂾</t>
+  </si>
+  <si>
+    <t>🃁</t>
+  </si>
+  <si>
+    <t>🃂</t>
+  </si>
+  <si>
+    <t>🃃</t>
+  </si>
+  <si>
+    <t>🃄</t>
+  </si>
+  <si>
+    <t>🃅</t>
+  </si>
+  <si>
+    <t>🃆</t>
+  </si>
+  <si>
+    <t>🃇</t>
+  </si>
+  <si>
+    <t>🃈</t>
+  </si>
+  <si>
+    <t>🃉</t>
+  </si>
+  <si>
+    <t>🃊</t>
+  </si>
+  <si>
+    <t>🃋</t>
+  </si>
+  <si>
+    <t>🃍</t>
+  </si>
+  <si>
+    <t>🃎</t>
+  </si>
+  <si>
+    <t>🂥</t>
+  </si>
+  <si>
+    <t>🂦</t>
+  </si>
+  <si>
+    <t>🂧</t>
+  </si>
+  <si>
+    <t>🂨</t>
+  </si>
+  <si>
+    <t>🂩</t>
+  </si>
+  <si>
+    <t>🂪</t>
+  </si>
+  <si>
+    <t>🂭</t>
+  </si>
+  <si>
+    <t>🂮</t>
+  </si>
+  <si>
+    <t>🃑</t>
+  </si>
+  <si>
+    <t>🃒</t>
+  </si>
+  <si>
+    <t>🃓</t>
+  </si>
+  <si>
+    <t>🃔</t>
+  </si>
+  <si>
+    <t>🃕</t>
+  </si>
+  <si>
+    <t>🃖</t>
+  </si>
+  <si>
+    <t>🃗</t>
+  </si>
+  <si>
+    <t>🃘</t>
+  </si>
+  <si>
+    <t>🃙</t>
+  </si>
+  <si>
+    <t>🃚</t>
+  </si>
+  <si>
+    <t>🃛</t>
+  </si>
+  <si>
+    <t>🃝</t>
+  </si>
+  <si>
+    <t>🃞</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDF000F"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF373637"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,8 +289,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,647 +610,1025 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216A1BF5-97D2-489B-A4A3-472319622C59}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="str">
-        <f>_xlfn.CONCAT($C$1,A3,", Value=CardValue.",B3,"});")</f>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT($D$1,A3,", Value=CardValue.",B3,"});")</f>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Ace});</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+      <c r="M3" t="str">
+        <f>_xlfn.CONCAT("case(CardNumber.",B3,", CardSuit.",A3,"): return """,C3,""";")</f>
+        <v>case(CardNumber.Ace, CardSuit.Heart): return "🂱";</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C54" si="0">_xlfn.CONCAT($C$1,A4,", Value=CardValue.",B4,"});")</f>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D54" si="0">_xlfn.CONCAT($D$1,A4,", Value=CardValue.",B4,"});")</f>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Two});</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M54" si="1">_xlfn.CONCAT("case(CardNumber.",B4,", CardSuit.",A4,"): return """,C4,""";")</f>
+        <v>case(CardNumber.Two, CardSuit.Heart): return "🂲";</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Three});</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Three, CardSuit.Heart): return "🂳";</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Four});</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Four, CardSuit.Heart): return "🂴";</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Five});</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Five, CardSuit.Heart): return "🂵";</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Six});</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Six, CardSuit.Heart): return "🂶";</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Seven});</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Seven, CardSuit.Heart): return "🂷";</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Eight});</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Eight, CardSuit.Heart): return "🂸";</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Nine});</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Nine, CardSuit.Heart): return "🂹";</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Ten});</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Ten, CardSuit.Heart): return "🂺";</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Jack});</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Jack, CardSuit.Heart): return "🂻";</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.Queen});</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Queen, CardSuit.Heart): return "🂽";</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Heart, Value=CardValue.King});</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.King, CardSuit.Heart): return "🂾";</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Ace});</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Ace, CardSuit.Diamond): return "🃁";</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Two});</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Two, CardSuit.Diamond): return "🃂";</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Three});</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Three, CardSuit.Diamond): return "🃃";</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Four});</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Four, CardSuit.Diamond): return "🃄";</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Five});</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Five, CardSuit.Diamond): return "🃅";</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Six});</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Six, CardSuit.Diamond): return "🃆";</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" t="str">
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Seven});</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Seven, CardSuit.Diamond): return "🃇";</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Eight});</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M23" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Eight, CardSuit.Diamond): return "🃈";</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C24" t="str">
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Nine});</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Nine, CardSuit.Diamond): return "🃉";</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Ten});</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M25" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Ten, CardSuit.Diamond): return "🃊";</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
       </c>
-      <c r="C26" t="str">
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Jack});</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M26" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Jack, CardSuit.Diamond): return "🃋";</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.Queen});</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M27" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Queen, CardSuit.Diamond): return "🃍";</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
       </c>
-      <c r="C28" t="str">
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Diamond, Value=CardValue.King});</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M28" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.King, CardSuit.Diamond): return "🃎";</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Ace});</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M29" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Ace, CardSuit.Spade): return "🂡";</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Two});</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M30" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Two, CardSuit.Spade): return "🂢";</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Three});</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M31" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Three, CardSuit.Spade): return "🂣";</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
-      <c r="C32" t="str">
+      <c r="C32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Four});</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M32" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Four, CardSuit.Spade): return "🂤";</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Five});</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M33" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Five, CardSuit.Spade): return "🂥";</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
       <c r="B34" t="s">
         <v>9</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Six});</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M34" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Six, CardSuit.Spade): return "🂦";</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
-      <c r="C35" t="str">
+      <c r="C35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Seven});</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M35" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Seven, CardSuit.Spade): return "🂧";</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Eight});</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M36" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Eight, CardSuit.Spade): return "🂨";</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Nine});</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M37" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Nine, CardSuit.Spade): return "🂩";</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
-      <c r="C38" t="str">
+      <c r="C38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Ten});</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M38" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Ten, CardSuit.Spade): return "🂪";</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Jack});</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M39" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Jack, CardSuit.Spade): return "🂪";</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1</v>
       </c>
       <c r="B40" t="s">
         <v>15</v>
       </c>
-      <c r="C40" t="str">
+      <c r="C40" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.Queen});</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M40" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Queen, CardSuit.Spade): return "🂭";</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
       <c r="B41" t="s">
         <v>16</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Spade, Value=CardValue.King});</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M41" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.King, CardSuit.Spade): return "🂮";</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
       </c>
-      <c r="C42" t="str">
+      <c r="C42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Ace});</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M42" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Ace, CardSuit.Club): return "🃑";</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>2</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Two});</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M43" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Two, CardSuit.Club): return "🃒";</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Three});</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M44" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Three, CardSuit.Club): return "🃓";</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>2</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Four});</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M45" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Four, CardSuit.Club): return "🃔";</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Five});</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M46" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Five, CardSuit.Club): return "🃕";</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>2</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Six});</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M47" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Six, CardSuit.Club): return "🃖";</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>2</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
-      <c r="C48" t="str">
+      <c r="C48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Seven});</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M48" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Seven, CardSuit.Club): return "🃗";</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>2</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Eight});</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M49" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Eight, CardSuit.Club): return "🃘";</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>2</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
       </c>
-      <c r="C50" t="str">
+      <c r="C50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Nine});</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M50" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Nine, CardSuit.Club): return "🃙";</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>2</v>
       </c>
       <c r="B51" t="s">
         <v>13</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Ten});</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M51" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Ten, CardSuit.Club): return "🃚";</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>2</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
       </c>
-      <c r="C52" t="str">
+      <c r="C52" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Jack});</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M52" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Jack, CardSuit.Club): return "🃛";</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>2</v>
       </c>
       <c r="B53" t="s">
         <v>15</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.Queen});</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M53" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.Queen, CardSuit.Club): return "🃝";</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>2</v>
       </c>
       <c r="B54" t="s">
         <v>16</v>
       </c>
-      <c r="C54" t="str">
+      <c r="C54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" t="str">
         <f t="shared" si="0"/>
         <v>cardsToTest.Add(new Card { Suit = CardSuit.Club, Value=CardValue.King});</v>
       </c>
+      <c r="M54" t="str">
+        <f t="shared" si="1"/>
+        <v>case(CardNumber.King, CardSuit.Club): return "🃞";</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4775407A-8ACD-4468-AEFB-30D0F02232B2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on adding support for bets, wip
</commit_message>
<xml_diff>
--- a/assets/cards.xlsx
+++ b/assets/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\mycode\blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B074071E-301B-423C-9C6A-8EF24443CF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B209B7C-C119-4321-90CD-2695D06F6C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{577205D3-06DB-45CE-85F4-7344C670B98B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{577205D3-06DB-45CE-85F4-7344C670B98B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="74">
   <si>
     <t>Diamond</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>(CardNumber.Ace, CardSuit.Heart) =&gt; "🂱",</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>cards.Add(new Card { Number = CardNumber.Ace, Suit = CardSuit.Heart });</t>
   </si>
 </sst>
 </file>
@@ -314,6 +326,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E4C95BB-46F2-4C00-ACBC-DD3D9BDFCF96}" name="Table1" displayName="Table1" ref="B2:D54" totalsRowShown="0">
+  <autoFilter ref="B2:D54" xr:uid="{2E4C95BB-46F2-4C00-ACBC-DD3D9BDFCF96}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D54">
+    <sortCondition ref="B2:B54"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DABE7E96-A53E-46A3-8007-66627D7794FC}" name="Column1">
+      <calculatedColumnFormula>RAND()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{F1048161-3E4E-477B-ACDD-332E03F9C57C}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{542F33D5-4A67-4FDD-BBB4-4A0CE02A2F9E}" name="Column3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216A1BF5-97D2-489B-A4A3-472319622C59}">
   <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3:S54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,12 +1866,869 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4775407A-8ACD-4468-AEFB-30D0F02232B2}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="4" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f ca="1">RAND()</f>
+        <v>0.23291787560243826</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Three, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f ca="1">RAND()</f>
+        <v>0.24790433622457786</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Six, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f ca="1">RAND()</f>
+        <v>0.26593081850009204</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Five, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f ca="1">RAND()</f>
+        <v>0.89869598750139201</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Three, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f ca="1">RAND()</f>
+        <v>0.2024243773519474</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ten, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f ca="1">RAND()</f>
+        <v>0.10944832631046164</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Six, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f ca="1">RAND()</f>
+        <v>0.82910252472574775</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Four, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f ca="1">RAND()</f>
+        <v>0.80195991539407396</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ace, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f ca="1">RAND()</f>
+        <v>0.74095565222151649</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ace, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f ca="1">RAND()</f>
+        <v>0.81961616241000157</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Four, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f ca="1">RAND()</f>
+        <v>0.41400434846911982</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Three, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f ca="1">RAND()</f>
+        <v>0.28655299173328952</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Six, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f ca="1">RAND()</f>
+        <v>0.72209491822251548</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Queen, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f ca="1">RAND()</f>
+        <v>0.56671817533434865</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ten, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f ca="1">RAND()</f>
+        <v>0.19130166661999648</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Three, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f ca="1">RAND()</f>
+        <v>2.4205850024084041E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Four, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f ca="1">RAND()</f>
+        <v>0.98848244294697085</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Two, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f ca="1">RAND()</f>
+        <v>0.2459653644418911</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Jack, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f ca="1">RAND()</f>
+        <v>0.35851746034654819</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Seven, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f ca="1">RAND()</f>
+        <v>0.77592986688875576</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Seven, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f ca="1">RAND()</f>
+        <v>0.67656007553564546</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Queen, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f ca="1">RAND()</f>
+        <v>0.87504412087307371</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Queen, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f ca="1">RAND()</f>
+        <v>0.56839546392394635</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ten, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f ca="1">RAND()</f>
+        <v>0.33229197290070889</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.King, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f ca="1">RAND()</f>
+        <v>0.17253056533039357</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ace, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f ca="1">RAND()</f>
+        <v>3.9416189989703088E-2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Six, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f ca="1">RAND()</f>
+        <v>0.65413194008058706</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Two, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f ca="1">RAND()</f>
+        <v>0.4446562819556048</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Two, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f ca="1">RAND()</f>
+        <v>0.74195473972151915</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Four, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f ca="1">RAND()</f>
+        <v>0.79950868481669501</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Eight, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f ca="1">RAND()</f>
+        <v>0.51494775977447338</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.King, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f ca="1">RAND()</f>
+        <v>0.55576469584912791</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Jack, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f ca="1">RAND()</f>
+        <v>0.63515713817595776</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Eight, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f ca="1">RAND()</f>
+        <v>0.57618936255041631</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Nine, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f ca="1">RAND()</f>
+        <v>0.4937194390052001</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Nine, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f ca="1">RAND()</f>
+        <v>0.7764165704003072</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Nine, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f ca="1">RAND()</f>
+        <v>0.52062927627800659</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Five, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f ca="1">RAND()</f>
+        <v>0.85273233392573133</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Eight, Suit=CardSuit.Spade});</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f ca="1">RAND()</f>
+        <v>3.9331801517880294E-2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ace, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f ca="1">RAND()</f>
+        <v>5.7171086224278023E-2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Jack, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f ca="1">RAND()</f>
+        <v>0.9035127217380986</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Nine, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f ca="1">RAND()</f>
+        <v>0.64811709350189872</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.King, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f ca="1">RAND()</f>
+        <v>0.32245033281621871</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Eight, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f ca="1">RAND()</f>
+        <v>0.57646396928556543</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Two, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f ca="1">RAND()</f>
+        <v>0.37247784617333579</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.King, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <f ca="1">RAND()</f>
+        <v>0.31500513269328623</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Ten, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f ca="1">RAND()</f>
+        <v>0.9761608785685747</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Queen, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <f ca="1">RAND()</f>
+        <v>0.85839824094769734</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Jack, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <f ca="1">RAND()</f>
+        <v>2.4149887086164612E-2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Five, Suit=CardSuit.Club});</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <f ca="1">RAND()</f>
+        <v>0.81405999146950492</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Seven, Suit=CardSuit.Heart});</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <f ca="1">RAND()</f>
+        <v>8.1671354642477767E-2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Seven, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <f ca="1">RAND()</f>
+        <v>0.38619025167141208</v>
+      </c>
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="str">
+        <f>_xlfn.CONCAT("cards.Add(new Card { Number=CardNumber.",Table1[[#This Row],[Column3]],", Suit=CardSuit.",Table1[[#This Row],[Column2]],"});")</f>
+        <v>cards.Add(new Card { Number=CardNumber.Five, Suit=CardSuit.Diamond});</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change to make NullLogger a singleton
</commit_message>
<xml_diff>
--- a/assets/cards.xlsx
+++ b/assets/cards.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\mycode\blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B209B7C-C119-4321-90CD-2695D06F6C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EE40E-D5C4-489D-993A-A8F26CE4DA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{577205D3-06DB-45CE-85F4-7344C670B98B}"/>
+    <workbookView xWindow="27940" yWindow="2660" windowWidth="10460" windowHeight="15820" activeTab="2" xr2:uid="{577205D3-06DB-45CE-85F4-7344C670B98B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="97">
   <si>
     <t>Diamond</t>
   </si>
@@ -257,6 +258,75 @@
   </si>
   <si>
     <t>cards.Add(new Card { Number = CardNumber.Ace, Suit = CardSuit.Heart });</t>
+  </si>
+  <si>
+    <t>CardNumberOrScore.</t>
+  </si>
+  <si>
+    <t>Busted</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Score21</t>
+  </si>
+  <si>
+    <t>Score20</t>
+  </si>
+  <si>
+    <t>Score19</t>
+  </si>
+  <si>
+    <t>Score18</t>
+  </si>
+  <si>
+    <t>Score17</t>
+  </si>
+  <si>
+    <t>Score16</t>
+  </si>
+  <si>
+    <t>Score15</t>
+  </si>
+  <si>
+    <t>Score14</t>
+  </si>
+  <si>
+    <t>Score13</t>
+  </si>
+  <si>
+    <t>Score12</t>
+  </si>
+  <si>
+    <t>Score11</t>
+  </si>
+  <si>
+    <t>Score10</t>
+  </si>
+  <si>
+    <t>Score9</t>
+  </si>
+  <si>
+    <t>Score8</t>
+  </si>
+  <si>
+    <t>Score7</t>
+  </si>
+  <si>
+    <t>Score6</t>
+  </si>
+  <si>
+    <t>Score5</t>
+  </si>
+  <si>
+    <t>Score4</t>
+  </si>
+  <si>
+    <t>Score3</t>
+  </si>
+  <si>
+    <t>Score2</t>
   </si>
 </sst>
 </file>
@@ -304,13 +374,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4775407A-8ACD-4468-AEFB-30D0F02232B2}">
   <dimension ref="B1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F54"/>
     </sheetView>
   </sheetViews>
@@ -1895,8 +1966,8 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
-        <f ca="1">RAND()</f>
-        <v>0.23291787560243826</v>
+        <f t="shared" ref="B3:B34" ca="1" si="0">RAND()</f>
+        <v>0.76799998868895381</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1911,8 +1982,8 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
-        <f ca="1">RAND()</f>
-        <v>0.24790433622457786</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.44239318694639262</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1927,8 +1998,8 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
-        <f ca="1">RAND()</f>
-        <v>0.26593081850009204</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33462363546854679</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1943,8 +2014,8 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
-        <f ca="1">RAND()</f>
-        <v>0.89869598750139201</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16565561309419063</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1959,8 +2030,8 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f ca="1">RAND()</f>
-        <v>0.2024243773519474</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7.8260618752491795E-2</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -1975,8 +2046,8 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
-        <f ca="1">RAND()</f>
-        <v>0.10944832631046164</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.83862983153951576</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -1991,8 +2062,8 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
-        <f ca="1">RAND()</f>
-        <v>0.82910252472574775</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80269501305415214</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -2007,8 +2078,8 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
-        <f ca="1">RAND()</f>
-        <v>0.80195991539407396</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.62513915873309767</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -2023,8 +2094,8 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f ca="1">RAND()</f>
-        <v>0.74095565222151649</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18822459967598804</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -2039,8 +2110,8 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
-        <f ca="1">RAND()</f>
-        <v>0.81961616241000157</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.62492430866195015</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -2055,8 +2126,8 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
-        <f ca="1">RAND()</f>
-        <v>0.41400434846911982</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61308967932652858</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
@@ -2071,8 +2142,8 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f ca="1">RAND()</f>
-        <v>0.28655299173328952</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.54977655625211397</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -2087,8 +2158,8 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
-        <f ca="1">RAND()</f>
-        <v>0.72209491822251548</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.40278988836778884</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -2103,8 +2174,8 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
-        <f ca="1">RAND()</f>
-        <v>0.56671817533434865</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.39153161234843303</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -2119,8 +2190,8 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
-        <f ca="1">RAND()</f>
-        <v>0.19130166661999648</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.37241882570927642</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -2135,8 +2206,8 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
-        <f ca="1">RAND()</f>
-        <v>2.4205850024084041E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68348012882060627</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -2151,8 +2222,8 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
-        <f ca="1">RAND()</f>
-        <v>0.98848244294697085</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.29754421979701506</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -2167,8 +2238,8 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f ca="1">RAND()</f>
-        <v>0.2459653644418911</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9607787846449044</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -2183,8 +2254,8 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f ca="1">RAND()</f>
-        <v>0.35851746034654819</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71193596117918345</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -2199,8 +2270,8 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f ca="1">RAND()</f>
-        <v>0.77592986688875576</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.28382427513764841</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -2215,8 +2286,8 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
-        <f ca="1">RAND()</f>
-        <v>0.67656007553564546</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69743826839145939</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -2231,8 +2302,8 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
-        <f ca="1">RAND()</f>
-        <v>0.87504412087307371</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.98201046333042408</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -2247,8 +2318,8 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
-        <f ca="1">RAND()</f>
-        <v>0.56839546392394635</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16310024867830542</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
@@ -2263,8 +2334,8 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
-        <f ca="1">RAND()</f>
-        <v>0.33229197290070889</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.31250934435195032</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -2279,8 +2350,8 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
-        <f ca="1">RAND()</f>
-        <v>0.17253056533039357</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.45817781909686273</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -2295,8 +2366,8 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
-        <f ca="1">RAND()</f>
-        <v>3.9416189989703088E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63206163947637328</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -2311,8 +2382,8 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
-        <f ca="1">RAND()</f>
-        <v>0.65413194008058706</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.45496546095298429</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -2327,8 +2398,8 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
-        <f ca="1">RAND()</f>
-        <v>0.4446562819556048</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34079902407799856</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2343,8 +2414,8 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
-        <f ca="1">RAND()</f>
-        <v>0.74195473972151915</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14976492245047601</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -2359,8 +2430,8 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
-        <f ca="1">RAND()</f>
-        <v>0.79950868481669501</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.57114337066832843</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
@@ -2375,8 +2446,8 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33">
-        <f ca="1">RAND()</f>
-        <v>0.51494775977447338</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.64279360637970573</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -2391,8 +2462,8 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
-        <f ca="1">RAND()</f>
-        <v>0.55576469584912791</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22294262452203173</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
@@ -2407,8 +2478,8 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35">
-        <f ca="1">RAND()</f>
-        <v>0.63515713817595776</v>
+        <f t="shared" ref="B35:B54" ca="1" si="1">RAND()</f>
+        <v>0.22930023830041524</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -2423,8 +2494,8 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36">
-        <f ca="1">RAND()</f>
-        <v>0.57618936255041631</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22235125556465463</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -2439,8 +2510,8 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37">
-        <f ca="1">RAND()</f>
-        <v>0.4937194390052001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.60320131269582455</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -2455,8 +2526,8 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38">
-        <f ca="1">RAND()</f>
-        <v>0.7764165704003072</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.96921513678019855</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -2471,8 +2542,8 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39">
-        <f ca="1">RAND()</f>
-        <v>0.52062927627800659</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4988722305654224</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -2487,8 +2558,8 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40">
-        <f ca="1">RAND()</f>
-        <v>0.85273233392573133</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31253386837899011</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -2503,8 +2574,8 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41">
-        <f ca="1">RAND()</f>
-        <v>3.9331801517880294E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.12258384671002631</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -2519,8 +2590,8 @@
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42">
-        <f ca="1">RAND()</f>
-        <v>5.7171086224278023E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77772928352447446</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -2535,8 +2606,8 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43">
-        <f ca="1">RAND()</f>
-        <v>0.9035127217380986</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.18034370910460251</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
@@ -2551,8 +2622,8 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44">
-        <f ca="1">RAND()</f>
-        <v>0.64811709350189872</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51198286566645312</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -2567,8 +2638,8 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45">
-        <f ca="1">RAND()</f>
-        <v>0.32245033281621871</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9580434981863255</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
@@ -2583,8 +2654,8 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46">
-        <f ca="1">RAND()</f>
-        <v>0.57646396928556543</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.62042091267911759</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
@@ -2599,8 +2670,8 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47">
-        <f ca="1">RAND()</f>
-        <v>0.37247784617333579</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68351075156605068</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -2615,8 +2686,8 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48">
-        <f ca="1">RAND()</f>
-        <v>0.31500513269328623</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15181940909802738</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -2631,8 +2702,8 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49">
-        <f ca="1">RAND()</f>
-        <v>0.9761608785685747</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88062761981998239</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
@@ -2647,8 +2718,8 @@
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50">
-        <f ca="1">RAND()</f>
-        <v>0.85839824094769734</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69426159710696334</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -2663,8 +2734,8 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51">
-        <f ca="1">RAND()</f>
-        <v>2.4149887086164612E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>8.2883685320671585E-2</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -2679,8 +2750,8 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52">
-        <f ca="1">RAND()</f>
-        <v>0.81405999146950492</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.39432238913291606</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
@@ -2695,8 +2766,8 @@
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53">
-        <f ca="1">RAND()</f>
-        <v>8.1671354642477767E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.8797700444727514E-2</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
@@ -2711,8 +2782,8 @@
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54">
-        <f ca="1">RAND()</f>
-        <v>0.38619025167141208</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.30405570461179066</v>
       </c>
       <c r="C54" t="s">
         <v>0</v>
@@ -2731,4 +2802,339 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072DC793-58AA-41B2-B8EA-0DB91639A55F}">
+  <dimension ref="B4:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="4">
+        <v>21</v>
+      </c>
+      <c r="G4" t="str">
+        <f>_xlfn.CONCAT(B4,C4,"=&gt; """, D4,""",")</f>
+        <v>CardNumberOrScore.Score21=&gt; "21",</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:G24" si="0">_xlfn.CONCAT(B5,C5,"=&gt; """, D5,""",")</f>
+        <v>CardNumberOrScore.Score20=&gt; "20",</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score19=&gt; "19",</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score18=&gt; "18",</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score17=&gt; "17",</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score16=&gt; "16",</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score15=&gt; "15",</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score14=&gt; "14",</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score13=&gt; "13",</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score12=&gt; "12",</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score11=&gt; "11",</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score10=&gt; "10",</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score9=&gt; "9",</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score8=&gt; "8",</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score7=&gt; "7",</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score6=&gt; "6",</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score5=&gt; "5",</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score4=&gt; "4",</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score3=&gt; "3",</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Score2=&gt; "2",</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>CardNumberOrScore.Busted=&gt; "B",</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sorting output for strategytree
</commit_message>
<xml_diff>
--- a/assets/cards.xlsx
+++ b/assets/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\mycode\blackjack\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EE40E-D5C4-489D-993A-A8F26CE4DA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B590CF7F-168C-4365-B826-BADF638583E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27940" yWindow="2660" windowWidth="10460" windowHeight="15820" activeTab="2" xr2:uid="{577205D3-06DB-45CE-85F4-7344C670B98B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{577205D3-06DB-45CE-85F4-7344C670B98B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="98">
   <si>
     <t>Diamond</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>Score2</t>
+  </si>
+  <si>
+    <t>CardNumberOrScore.Ace =&gt; 11,</t>
   </si>
 </sst>
 </file>
@@ -716,7 +719,7 @@
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B54"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1970,7 @@
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <f t="shared" ref="B3:B34" ca="1" si="0">RAND()</f>
-        <v>0.76799998868895381</v>
+        <v>0.34082739176656773</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1983,7 +1986,7 @@
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44239318694639262</v>
+        <v>0.57480632060101078</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1999,7 +2002,7 @@
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33462363546854679</v>
+        <v>9.6165990374513455E-2</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -2015,7 +2018,7 @@
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16565561309419063</v>
+        <v>0.35881411436911748</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -2031,7 +2034,7 @@
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>7.8260618752491795E-2</v>
+        <v>0.98374266395644117</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -2047,7 +2050,7 @@
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83862983153951576</v>
+        <v>0.46264752965120282</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -2063,7 +2066,7 @@
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80269501305415214</v>
+        <v>0.55854049767475711</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -2079,7 +2082,7 @@
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62513915873309767</v>
+        <v>6.1605458518871448E-2</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -2095,7 +2098,7 @@
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18822459967598804</v>
+        <v>0.40996019885713419</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -2111,7 +2114,7 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62492430866195015</v>
+        <v>0.71818531251501327</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -2127,7 +2130,7 @@
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61308967932652858</v>
+        <v>0.27763653051552117</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
@@ -2143,7 +2146,7 @@
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54977655625211397</v>
+        <v>0.39521294015559028</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -2159,7 +2162,7 @@
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40278988836778884</v>
+        <v>6.6451850507511456E-2</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -2175,7 +2178,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39153161234843303</v>
+        <v>0.5138915339604887</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -2191,7 +2194,7 @@
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37241882570927642</v>
+        <v>0.26478241857400131</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -2207,7 +2210,7 @@
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68348012882060627</v>
+        <v>0.27552781306083352</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -2223,7 +2226,7 @@
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29754421979701506</v>
+        <v>0.57516599545972058</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -2239,7 +2242,7 @@
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9607787846449044</v>
+        <v>0.72425106800873695</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -2255,7 +2258,7 @@
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71193596117918345</v>
+        <v>0.14696655930962954</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -2271,7 +2274,7 @@
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28382427513764841</v>
+        <v>0.8281874854115826</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -2287,7 +2290,7 @@
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69743826839145939</v>
+        <v>0.24230987392465642</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -2303,7 +2306,7 @@
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98201046333042408</v>
+        <v>0.30782390231586476</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -2319,7 +2322,7 @@
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16310024867830542</v>
+        <v>0.3480310341833327</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
@@ -2335,7 +2338,7 @@
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31250934435195032</v>
+        <v>0.98239333043660215</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -2351,7 +2354,7 @@
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45817781909686273</v>
+        <v>0.38703982994925601</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -2367,7 +2370,7 @@
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63206163947637328</v>
+        <v>0.96088972861541067</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -2383,7 +2386,7 @@
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45496546095298429</v>
+        <v>0.41247215664056103</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -2399,7 +2402,7 @@
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34079902407799856</v>
+        <v>0.13077519374033952</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2415,7 +2418,7 @@
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14976492245047601</v>
+        <v>0.23082326300629408</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -2431,7 +2434,7 @@
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57114337066832843</v>
+        <v>0.70401026902479757</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
@@ -2447,7 +2450,7 @@
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64279360637970573</v>
+        <v>0.45239590519582662</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -2463,7 +2466,7 @@
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22294262452203173</v>
+        <v>0.50721996235964262</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
@@ -2479,7 +2482,7 @@
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" ref="B35:B54" ca="1" si="1">RAND()</f>
-        <v>0.22930023830041524</v>
+        <v>0.12316719665529186</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -2495,7 +2498,7 @@
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22235125556465463</v>
+        <v>0.91444655814382858</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -2511,7 +2514,7 @@
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60320131269582455</v>
+        <v>0.4442610997589469</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -2527,7 +2530,7 @@
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.96921513678019855</v>
+        <v>6.4872266359182307E-2</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
@@ -2543,7 +2546,7 @@
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4988722305654224</v>
+        <v>2.3457575658257346E-2</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -2559,7 +2562,7 @@
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31253386837899011</v>
+        <v>0.74576669507127036</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -2575,7 +2578,7 @@
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12258384671002631</v>
+        <v>0.83473583832253784</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -2591,7 +2594,7 @@
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.77772928352447446</v>
+        <v>7.4751421237400639E-2</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -2607,7 +2610,7 @@
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18034370910460251</v>
+        <v>0.21095350985316275</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
@@ -2623,7 +2626,7 @@
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51198286566645312</v>
+        <v>0.80617932939146575</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -2639,7 +2642,7 @@
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9580434981863255</v>
+        <v>0.41582253373866596</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
@@ -2655,7 +2658,7 @@
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62042091267911759</v>
+        <v>0.13264165417078388</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
@@ -2671,7 +2674,7 @@
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68351075156605068</v>
+        <v>0.74687938494608264</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -2687,7 +2690,7 @@
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15181940909802738</v>
+        <v>0.84547799516771216</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -2703,7 +2706,7 @@
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88062761981998239</v>
+        <v>0.14622582784675953</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
@@ -2719,7 +2722,7 @@
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69426159710696334</v>
+        <v>8.4095992233096828E-2</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -2735,7 +2738,7 @@
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2883685320671585E-2</v>
+        <v>0.49136913371769397</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -2751,7 +2754,7 @@
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39432238913291606</v>
+        <v>0.26806289114911475</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
@@ -2767,7 +2770,7 @@
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8797700444727514E-2</v>
+        <v>0.99958725711505025</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
@@ -2783,7 +2786,7 @@
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30405570461179066</v>
+        <v>0.40487178028484105</v>
       </c>
       <c r="C54" t="s">
         <v>0</v>
@@ -2806,10 +2809,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072DC793-58AA-41B2-B8EA-0DB91639A55F}">
-  <dimension ref="B4:G24"/>
+  <dimension ref="B4:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,7 +3017,7 @@
         <v>CardNumberOrScore.Score9=&gt; "9",</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>74</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>CardNumberOrScore.Score8=&gt; "8",</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>74</v>
       </c>
@@ -3044,7 +3047,7 @@
         <v>CardNumberOrScore.Score7=&gt; "7",</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>74</v>
       </c>
@@ -3059,7 +3062,7 @@
         <v>CardNumberOrScore.Score6=&gt; "6",</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>74</v>
       </c>
@@ -3074,7 +3077,7 @@
         <v>CardNumberOrScore.Score5=&gt; "5",</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>74</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>CardNumberOrScore.Score4=&gt; "4",</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>74</v>
       </c>
@@ -3104,7 +3107,7 @@
         <v>CardNumberOrScore.Score3=&gt; "3",</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>74</v>
       </c>
@@ -3119,7 +3122,7 @@
         <v>CardNumberOrScore.Score2=&gt; "2",</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>74</v>
       </c>
@@ -3132,6 +3135,521 @@
       <c r="G24" t="str">
         <f t="shared" si="0"/>
         <v>CardNumberOrScore.Busted=&gt; "B",</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+      <c r="G27" t="str">
+        <f>_xlfn.CONCAT(B27,C27," =&gt; ",E27,",")</f>
+        <v>CardNumberOrScore.Ace =&gt; 11,</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" ref="G28:G60" si="1">_xlfn.CONCAT(B28,C28," =&gt; ",E28,",")</f>
+        <v>CardNumberOrScore.Two =&gt; 2,</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Three =&gt; 3,</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Four =&gt; 4,</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Five =&gt; 5,</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Six =&gt; 6,</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Seven =&gt; 7,</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Eight =&gt; 8,</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>9</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Nine =&gt; 9,</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Ten =&gt; 10,</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Jack =&gt; 10,</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Queen =&gt; 10,</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.King =&gt; 10,</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="4">
+        <v>21</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score21 =&gt; 21,</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score20 =&gt; 20,</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42">
+        <v>19</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score19 =&gt; 19,</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43">
+        <v>18</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score18 =&gt; 18,</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44">
+        <v>17</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score17 =&gt; 17,</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score16 =&gt; 16,</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46">
+        <v>15</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score15 =&gt; 15,</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47">
+        <v>14</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score14 =&gt; 14,</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48">
+        <v>13</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score13 =&gt; 13,</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49">
+        <v>12</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score12 =&gt; 12,</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50">
+        <v>11</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score11 =&gt; 11,</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51">
+        <v>10</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score10 =&gt; 10,</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52">
+        <v>9</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score9 =&gt; 9,</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score8 =&gt; 8,</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54">
+        <v>7</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score7 =&gt; 7,</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score6 =&gt; 6,</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score5 =&gt; 5,</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score4 =&gt; 4,</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score3 =&gt; 3,</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Score2 =&gt; 2,</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60">
+        <v>22</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="1"/>
+        <v>CardNumberOrScore.Busted =&gt; 22,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>